<commit_message>
2nd commit by Somnath Baul
</commit_message>
<xml_diff>
--- a/CommonData.xlsx
+++ b/CommonData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Somnath Baul\eclipse-workspace\MobileSeeTestWebAutomation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AE1AE10-D621-42B2-BAA8-11E42475268C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DC6121D-BC99-4C67-97D3-00384872F979}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{DB6BE804-BEA8-484A-ABCF-DE73BAEA4474}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{DB6BE804-BEA8-484A-ABCF-DE73BAEA4474}"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="UpdateMyAccount" sheetId="3" r:id="rId3"/>
     <sheet name="LoggedInOrder" sheetId="5" r:id="rId4"/>
     <sheet name="AddMyVisit" sheetId="4" r:id="rId5"/>
+    <sheet name="CarryOut" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="44">
   <si>
     <t>UserName</t>
   </si>
@@ -142,6 +143,33 @@
   </si>
   <si>
     <t>Somnath</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>145</t>
+  </si>
+  <si>
+    <t>2025</t>
+  </si>
+  <si>
+    <t>75001</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>Pickup Time</t>
+  </si>
+  <si>
+    <t>2018</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>11:30 AM</t>
   </si>
 </sst>
 </file>
@@ -517,7 +545,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{312E5F7E-74EE-4A19-968B-2855B98CC147}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -637,7 +665,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -689,23 +717,23 @@
       <c r="C2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="3">
-        <v>145</v>
-      </c>
-      <c r="E2" s="3">
-        <v>4</v>
-      </c>
-      <c r="F2" s="3">
-        <v>2025</v>
+      <c r="D2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="H2" s="3">
-        <v>75001</v>
-      </c>
-      <c r="I2" s="3">
-        <v>15</v>
+      <c r="H2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -719,7 +747,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -763,21 +791,50 @@
       <c r="C2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="3">
-        <v>4</v>
-      </c>
-      <c r="E2" s="3">
-        <v>2018</v>
+      <c r="D2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="3">
-        <v>20</v>
+      <c r="G2" s="3" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF536E93-01FA-4B0C-BA01-C1511D75F062}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N15" sqref="N15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fifth commit by Somnath Baul
</commit_message>
<xml_diff>
--- a/CommonData.xlsx
+++ b/CommonData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Somnath Baul\eclipse-workspace\MobileSeeTestWebAutomation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DC6121D-BC99-4C67-97D3-00384872F979}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF82A21E-7AE4-48AD-BB22-35E6E609FC4F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{DB6BE804-BEA8-484A-ABCF-DE73BAEA4474}"/>
+    <workbookView xWindow="2616" yWindow="2616" windowWidth="17280" windowHeight="8964" firstSheet="3" activeTab="7" xr2:uid="{DB6BE804-BEA8-484A-ABCF-DE73BAEA4474}"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,9 @@
     <sheet name="LoggedInOrder" sheetId="5" r:id="rId4"/>
     <sheet name="AddMyVisit" sheetId="4" r:id="rId5"/>
     <sheet name="CarryOut" sheetId="6" r:id="rId6"/>
+    <sheet name="Menu" sheetId="7" r:id="rId7"/>
+    <sheet name="DeliveryASAP" sheetId="8" r:id="rId8"/>
+    <sheet name="GuestUserCurbSide" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="59">
   <si>
     <t>UserName</t>
   </si>
@@ -170,6 +173,51 @@
   </si>
   <si>
     <t>11:30 AM</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Appetizers</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>Southwestern Eggrolls</t>
+  </si>
+  <si>
+    <t>Test1</t>
+  </si>
+  <si>
+    <t>Data1</t>
+  </si>
+  <si>
+    <t>Contact Number</t>
+  </si>
+  <si>
+    <t>abcd@qmail.com</t>
+  </si>
+  <si>
+    <t>Vehicle Make</t>
+  </si>
+  <si>
+    <t>Toyota</t>
+  </si>
+  <si>
+    <t>Vehicle Model</t>
+  </si>
+  <si>
+    <t>E1346</t>
+  </si>
+  <si>
+    <t>Vehicle Color</t>
+  </si>
+  <si>
+    <t>Blue</t>
+  </si>
+  <si>
+    <t>(512)242-3434</t>
   </si>
 </sst>
 </file>
@@ -814,7 +862,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF536E93-01FA-4B0C-BA01-C1511D75F062}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
@@ -837,4 +885,133 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FECA2BF-3040-4BEA-B090-52B1B931C11E}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B136618-5F2E-4D23-9367-FFAF27BCCCFF}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{4CDFF9E2-D64A-49BD-9C0A-2DB33AFE3185}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEEFE299-A6B3-4915-B70B-B8260F09A244}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
sixth push by Somnath Baul
</commit_message>
<xml_diff>
--- a/CommonData.xlsx
+++ b/CommonData.xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Somnath Baul\eclipse-workspace\MobileSeeTestWebAutomation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF82A21E-7AE4-48AD-BB22-35E6E609FC4F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C4D6F7B-2B4F-41F8-9C62-D9DEEBB1FEA9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2616" yWindow="2616" windowWidth="17280" windowHeight="8964" firstSheet="3" activeTab="7" xr2:uid="{DB6BE804-BEA8-484A-ABCF-DE73BAEA4474}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="8" xr2:uid="{DB6BE804-BEA8-484A-ABCF-DE73BAEA4474}"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
     <sheet name="Locations" sheetId="2" r:id="rId2"/>
     <sheet name="UpdateMyAccount" sheetId="3" r:id="rId3"/>
     <sheet name="LoggedInOrder" sheetId="5" r:id="rId4"/>
-    <sheet name="AddMyVisit" sheetId="4" r:id="rId5"/>
-    <sheet name="CarryOut" sheetId="6" r:id="rId6"/>
-    <sheet name="Menu" sheetId="7" r:id="rId7"/>
-    <sheet name="DeliveryASAP" sheetId="8" r:id="rId8"/>
-    <sheet name="GuestUserCurbSide" sheetId="9" r:id="rId9"/>
+    <sheet name="ReOrder" sheetId="10" r:id="rId5"/>
+    <sheet name="AddMyVisit" sheetId="4" r:id="rId6"/>
+    <sheet name="CarryOut" sheetId="6" r:id="rId7"/>
+    <sheet name="Menu" sheetId="7" r:id="rId8"/>
+    <sheet name="DeliveryASAP" sheetId="8" r:id="rId9"/>
+    <sheet name="GuestUserCurbSide" sheetId="9" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="71">
   <si>
     <t>UserName</t>
   </si>
@@ -218,6 +219,42 @@
   </si>
   <si>
     <t>(512)242-3434</t>
+  </si>
+  <si>
+    <t>Restaurant Address</t>
+  </si>
+  <si>
+    <t>16623 Coit Road, Dallas, TX 75248, USA</t>
+  </si>
+  <si>
+    <t>Apt. no</t>
+  </si>
+  <si>
+    <t>Instruction</t>
+  </si>
+  <si>
+    <t>Anything</t>
+  </si>
+  <si>
+    <t>Delray Beach, FL, USA</t>
+  </si>
+  <si>
+    <t>delray-beach</t>
+  </si>
+  <si>
+    <t>Mix &amp; Match Fajitas</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>14534 South Military Trail Delray Beach, FL 33484, USA</t>
+  </si>
+  <si>
+    <t>23</t>
   </si>
 </sst>
 </file>
@@ -271,11 +308,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -627,12 +665,54 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEEFE299-A6B3-4915-B70B-B8260F09A244}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCB0259F-0340-495B-8CB1-E9149FFADBF7}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -647,6 +727,11 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>5</v>
       </c>
     </row>
@@ -710,15 +795,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DACE546-71A1-4E6D-A325-3C92C533B150}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.21875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.21875" bestFit="1" customWidth="1"/>
@@ -756,11 +841,11 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>26</v>
+      <c r="A2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" t="s">
+        <v>66</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>28</v>
@@ -782,6 +867,14 @@
       </c>
       <c r="I2" s="3" t="s">
         <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -791,6 +884,32 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD9B41C5-87FA-4C7B-BB08-3689826904B3}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B08B26BE-501E-493E-AB72-741DFD0D9FA4}">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -858,7 +977,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF536E93-01FA-4B0C-BA01-C1511D75F062}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -887,7 +1006,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FECA2BF-3040-4BEA-B090-52B1B931C11E}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -922,12 +1041,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B136618-5F2E-4D23-9367-FFAF27BCCCFF}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -936,34 +1055,59 @@
     <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="46.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="E1" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="4" t="s">
         <v>51</v>
+      </c>
+      <c r="E2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E3" s="3" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -971,47 +1115,6 @@
     <hyperlink ref="D2" r:id="rId1" xr:uid="{4CDFF9E2-D64A-49BD-9C0A-2DB33AFE3185}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEEFE299-A6B3-4915-B70B-B8260F09A244}">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.77734375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Eighth push by Somnath
</commit_message>
<xml_diff>
--- a/CommonData.xlsx
+++ b/CommonData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Somnath Baul\eclipse-workspace\MobileSeeTestWebAutomation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C4D6F7B-2B4F-41F8-9C62-D9DEEBB1FEA9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06DE146C-6D3C-4B0F-A4B6-886B92EE0EFB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="8" xr2:uid="{DB6BE804-BEA8-484A-ABCF-DE73BAEA4474}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="1" xr2:uid="{DB6BE804-BEA8-484A-ABCF-DE73BAEA4474}"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
@@ -711,8 +711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCB0259F-0340-495B-8CB1-E9149FFADBF7}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1045,7 +1045,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B136618-5F2E-4D23-9367-FFAF27BCCCFF}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Ninth commit by Somnath Baul 14/06/21
</commit_message>
<xml_diff>
--- a/CommonData.xlsx
+++ b/CommonData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Somnath Baul\eclipse-workspace\MobileSeeTestWebAutomation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06DE146C-6D3C-4B0F-A4B6-886B92EE0EFB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDD30CAA-B112-42EA-95AE-1CC8C36A1901}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="1" xr2:uid="{DB6BE804-BEA8-484A-ABCF-DE73BAEA4474}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{DB6BE804-BEA8-484A-ABCF-DE73BAEA4474}"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,8 @@
     <sheet name="Menu" sheetId="7" r:id="rId8"/>
     <sheet name="DeliveryASAP" sheetId="8" r:id="rId9"/>
     <sheet name="GuestUserCurbSide" sheetId="9" r:id="rId10"/>
+    <sheet name="Delivery" sheetId="11" r:id="rId11"/>
+    <sheet name="Order Customization" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="80">
   <si>
     <t>UserName</t>
   </si>
@@ -74,18 +76,6 @@
     <t>Zip Code</t>
   </si>
   <si>
-    <t>Ramesh2</t>
-  </si>
-  <si>
-    <t>Sarkar2</t>
-  </si>
-  <si>
-    <t>somnath.baul123@brinker.com</t>
-  </si>
-  <si>
-    <t>75090</t>
-  </si>
-  <si>
     <t>Chilis Location from DropDown</t>
   </si>
   <si>
@@ -255,6 +245,45 @@
   </si>
   <si>
     <t>23</t>
+  </si>
+  <si>
+    <t>Delivery Date</t>
+  </si>
+  <si>
+    <t>Later Today</t>
+  </si>
+  <si>
+    <t>Delivery Time</t>
+  </si>
+  <si>
+    <t>Custom Item</t>
+  </si>
+  <si>
+    <t>Avocado-Ranch Dressing</t>
+  </si>
+  <si>
+    <t>Oldtimer with Cheese</t>
+  </si>
+  <si>
+    <t>Crispy Honey-Chipotle Chicken Crispers</t>
+  </si>
+  <si>
+    <t>Smokehouse Combo</t>
+  </si>
+  <si>
+    <t>ChilisFavourites</t>
+  </si>
+  <si>
+    <t>Ramesh5</t>
+  </si>
+  <si>
+    <t>Sarkar5</t>
+  </si>
+  <si>
+    <t>somnath.baul12345@brinker.com</t>
+  </si>
+  <si>
+    <t>75099</t>
   </si>
 </sst>
 </file>
@@ -308,12 +337,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="19" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -682,24 +713,87 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" t="s">
         <v>52</v>
-      </c>
-      <c r="B1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C1" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" t="s">
         <v>53</v>
       </c>
-      <c r="B2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C2" t="s">
-        <v>57</v>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBCECCC7-9998-469D-BB8C-640A40CD297A}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" s="5">
+        <v>0.52083333333333337</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB125B6C-A77D-4F44-8A9A-7803AC20D8CF}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -711,7 +805,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCB0259F-0340-495B-8CB1-E9149FFADBF7}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -727,7 +821,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
@@ -745,7 +839,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB347A0A-96B2-46B0-9301-4D003963C523}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -772,16 +866,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>76</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>77</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>12</v>
+        <v>78</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>13</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -813,68 +907,68 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
         <v>23</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>25</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>27</v>
       </c>
-      <c r="D1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E1" t="s">
-        <v>31</v>
-      </c>
       <c r="F1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="H1" t="s">
         <v>9</v>
       </c>
       <c r="I1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -888,19 +982,19 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -930,22 +1024,22 @@
         <v>4</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="F1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -953,22 +1047,22 @@
         <v>5</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -992,12 +1086,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1008,32 +1102,59 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FECA2BF-3040-4BEA-B090-52B1B931C11E}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B2" t="s">
-        <v>47</v>
+        <v>43</v>
+      </c>
+      <c r="C2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1067,47 +1188,47 @@
         <v>7</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E3" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Commit by somnath as on 16/06/2021
</commit_message>
<xml_diff>
--- a/CommonData.xlsx
+++ b/CommonData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Somnath Baul\eclipse-workspace\MobileSeeTestWebAutomation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDD30CAA-B112-42EA-95AE-1CC8C36A1901}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD13753A-625B-49AD-B065-8AFB3BA75392}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{DB6BE804-BEA8-484A-ABCF-DE73BAEA4474}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{DB6BE804-BEA8-484A-ABCF-DE73BAEA4474}"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
@@ -25,6 +25,7 @@
     <sheet name="GuestUserCurbSide" sheetId="9" r:id="rId10"/>
     <sheet name="Delivery" sheetId="11" r:id="rId11"/>
     <sheet name="Order Customization" sheetId="12" r:id="rId12"/>
+    <sheet name="OrderWithRewards" sheetId="13" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="82">
   <si>
     <t>UserName</t>
   </si>
@@ -284,6 +285,12 @@
   </si>
   <si>
     <t>75099</t>
+  </si>
+  <si>
+    <t>Reward Item</t>
+  </si>
+  <si>
+    <t>Chips and Salsa</t>
   </si>
 </sst>
 </file>
@@ -801,12 +808,38 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3E730BB-7902-43AD-B49A-2859F94FCDCC}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCB0259F-0340-495B-8CB1-E9149FFADBF7}">
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -821,12 +854,12 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>60</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -839,7 +872,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB347A0A-96B2-46B0-9301-4D003963C523}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -891,8 +924,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DACE546-71A1-4E6D-A325-3C92C533B150}">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -935,8 +968,8 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>61</v>
+      <c r="A2" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="B2" t="s">
         <v>62</v>
@@ -964,8 +997,8 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>20</v>
+      <c r="A3" t="s">
+        <v>61</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>22</v>

</xml_diff>